<commit_message>
EPBDS-6830 Implement circular datatype dependencies support like in Java.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7084_external_Datatypes.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7084_external_Datatypes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DD669D-E337-44A3-8C67-695CB7F6D672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5760" windowWidth="14895" windowHeight="2340" tabRatio="965" activeTab="3"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="965" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="93" r:id="rId1"/>
@@ -25,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yury Molchan</author>
   </authors>
   <commentList>
-    <comment ref="K29" authorId="0">
+    <comment ref="K29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -62,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="83">
   <si>
     <t>String</t>
   </si>
@@ -239,9 +245,6 @@
   </si>
   <si>
     <t>Method BeanA proxyA(BeanA bean)</t>
-  </si>
-  <si>
-    <t>MyTXT</t>
   </si>
   <si>
     <t>_PK_</t>
@@ -319,7 +322,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -487,21 +490,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
-    <cellStyle name="Comma 2" xfId="2"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="5" builtinId="10"/>
-    <cellStyle name="Output" xfId="6" builtinId="21"/>
-    <cellStyle name="Обычный 6" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Вывод" xfId="6" builtinId="21"/>
+    <cellStyle name="Вычисление" xfId="4" builtinId="22"/>
+    <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Примечание" xfId="5" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -518,14 +521,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -563,9 +569,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -598,9 +604,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -633,9 +656,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -808,28 +848,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B4" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -840,7 +880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -851,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -862,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -873,7 +913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -884,7 +924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
@@ -895,7 +935,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -906,7 +946,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
@@ -917,14 +957,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B16" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
@@ -935,7 +975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,14 +986,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
@@ -964,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
@@ -975,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
@@ -986,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
@@ -997,7 +1037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1008,7 +1048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1059,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
@@ -1030,14 +1070,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B33" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="2:4" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,89 +1100,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B3" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B9" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B22" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B27" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B28" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
@@ -1153,20 +1193,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="18" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B3" s="6" t="s">
         <v>54</v>
       </c>
@@ -1185,7 +1225,7 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
@@ -1232,7 +1272,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1279,7 +1319,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1298,7 +1338,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1312,28 +1352,28 @@
         <v>7777777</v>
       </c>
       <c r="J7" s="1">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="K7" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="L7" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="M7" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="N7" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="O7" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="P7" s="1">
         <v>7777777</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
@@ -1350,25 +1390,25 @@
         <v>7777777</v>
       </c>
       <c r="K8" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="L8" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="M8" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="N8" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="O8" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="P8" s="1">
-        <v>64000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B9" s="4" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1455,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B12" s="6" t="s">
         <v>55</v>
       </c>
@@ -1436,7 +1476,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1489,7 +1529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1542,7 +1582,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
@@ -1563,7 +1603,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
@@ -1578,31 +1618,31 @@
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="L16" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="M16" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="N16" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="O16" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="P16" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="Q16" s="1">
         <v>7777777</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B17" s="4" t="s">
         <v>42</v>
       </c>
@@ -1620,28 +1660,28 @@
         <v>7777777</v>
       </c>
       <c r="L17" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="M17" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="N17" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="O17" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="P17" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="Q17" s="1">
-        <v>64000</v>
+        <v>64</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B18" s="4" t="s">
         <v>43</v>
       </c>
@@ -1694,7 +1734,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B21" s="6" t="s">
         <v>23</v>
       </c>
@@ -1713,7 +1753,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1760,7 +1800,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B23" s="4" t="s">
         <v>16</v>
       </c>
@@ -1807,7 +1847,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B24" s="4" t="s">
         <v>17</v>
       </c>
@@ -1826,7 +1866,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1861,7 +1901,7 @@
         <v>7777777</v>
       </c>
     </row>
-    <row r="26" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B26" s="4" t="s">
         <v>42</v>
       </c>
@@ -1896,7 +1936,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B27" s="4" t="s">
         <v>43</v>
       </c>
@@ -1943,7 +1983,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B30" s="6" t="s">
         <v>41</v>
       </c>
@@ -1964,7 +2004,7 @@
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -2017,7 +2057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B32" s="4" t="s">
         <v>16</v>
       </c>
@@ -2070,7 +2110,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B33" s="4" t="s">
         <v>17</v>
       </c>
@@ -2091,7 +2131,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B34" s="4" t="s">
         <v>18</v>
       </c>
@@ -2130,7 +2170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B35" s="4" t="s">
         <v>42</v>
       </c>
@@ -2169,7 +2209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B36" s="4" t="s">
         <v>43</v>
       </c>
@@ -2222,9 +2262,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B39" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -2241,7 +2281,7 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.5">
       <c r="B40" s="2" t="s">
         <v>24</v>
       </c>
@@ -2288,7 +2328,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B41" s="4" t="s">
         <v>16</v>
       </c>
@@ -2335,7 +2375,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B42" s="4" t="s">
         <v>17</v>
       </c>
@@ -2354,7 +2394,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B43" s="4" t="s">
         <v>18</v>
       </c>
@@ -2389,7 +2429,7 @@
         <v>7777777</v>
       </c>
     </row>
-    <row r="44" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B44" s="4" t="s">
         <v>42</v>
       </c>
@@ -2424,7 +2464,7 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="45" spans="2:18" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:18" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B45" s="4" t="s">
         <v>43</v>
       </c>
@@ -2484,14 +2524,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="9" width="9.5703125" customWidth="1"/>
@@ -2500,9 +2540,9 @@
     <col min="15" max="22" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -2516,7 +2556,7 @@
       </c>
       <c r="L3" s="6"/>
       <c r="N3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -2531,9 +2571,9 @@
       </c>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -2557,13 +2597,13 @@
         <v>8</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="N4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>2</v>
@@ -2590,13 +2630,13 @@
         <v>13</v>
       </c>
       <c r="X4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Y4" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
@@ -2622,10 +2662,10 @@
         <v>8</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N5" s="4" t="s">
         <v>16</v>
@@ -2655,13 +2695,13 @@
         <v>13</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2673,10 +2713,10 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="K6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>17</v>
@@ -2690,13 +2730,13 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="X6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Y6" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2713,7 +2753,7 @@
         <v>17</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>18</v>
@@ -2732,10 +2772,10 @@
         <v>17</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
@@ -2752,7 +2792,7 @@
         <v>18</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>42</v>
@@ -2771,10 +2811,10 @@
         <v>18</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B9" s="4" t="s">
         <v>43</v>
       </c>
@@ -2803,7 +2843,7 @@
         <v>42</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>43</v>
@@ -2836,12 +2876,12 @@
         <v>42</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2854,10 +2894,10 @@
         <v>43</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -2871,118 +2911,118 @@
         <v>43</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="H11" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="I11" s="1">
         <v>7777777</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O11" s="1">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="P11" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="R11" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="S11" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="T11" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="U11" s="1">
         <v>7777777</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1">
         <v>7777777</v>
       </c>
       <c r="D12" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="F12" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="H12" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="I12" s="1">
-        <v>64000</v>
+        <v>64</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O12" s="1">
         <v>7777777</v>
       </c>
       <c r="P12" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="R12" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="S12" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="T12" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="U12" s="1">
-        <v>64000</v>
+        <v>64</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1">
         <v>128</v>
@@ -3006,7 +3046,7 @@
         <v>8192</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O13" s="1">
         <v>128</v>
@@ -3033,9 +3073,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -3048,25 +3088,25 @@
         <v>23</v>
       </c>
       <c r="L16" s="6"/>
-      <c r="N16" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
+      <c r="N16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
       <c r="X16" s="6" t="s">
         <v>41</v>
       </c>
       <c r="Y16" s="6"/>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
@@ -3090,13 +3130,13 @@
         <v>8</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="N17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>2</v>
@@ -3123,13 +3163,13 @@
         <v>13</v>
       </c>
       <c r="X17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Y17" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
@@ -3155,10 +3195,10 @@
         <v>8</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>16</v>
@@ -3188,13 +3228,13 @@
         <v>13</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
@@ -3206,10 +3246,10 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="K19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>17</v>
@@ -3223,13 +3263,13 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="X19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y19" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Y19" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
@@ -3246,7 +3286,7 @@
         <v>17</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>18</v>
@@ -3265,10 +3305,10 @@
         <v>17</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
@@ -3285,7 +3325,7 @@
         <v>18</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N21" s="4" t="s">
         <v>42</v>
@@ -3304,10 +3344,10 @@
         <v>18</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
@@ -3336,7 +3376,7 @@
         <v>42</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>43</v>
@@ -3369,12 +3409,12 @@
         <v>42</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B23" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -3387,10 +3427,10 @@
         <v>43</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -3404,12 +3444,12 @@
         <v>43</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -3433,7 +3473,7 @@
         <v>7777777</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O24" s="1">
         <v>1</v>
@@ -3460,9 +3500,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B25" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1">
         <v>7777777</v>
@@ -3486,7 +3526,7 @@
         <v>64</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O25" s="1">
         <v>7777777</v>
@@ -3513,9 +3553,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1">
         <v>128</v>
@@ -3539,7 +3579,7 @@
         <v>8192</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O26" s="1">
         <v>128</v>
@@ -3566,9 +3606,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B29" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -3577,14 +3617,14 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-      <c r="K29" s="8" t="s">
+      <c r="K29" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.5">
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>2</v>
@@ -3608,13 +3648,13 @@
         <v>8</v>
       </c>
       <c r="K30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B31" s="4" t="s">
         <v>16</v>
       </c>
@@ -3640,13 +3680,13 @@
         <v>8</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="2:25" ht="15.75" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B32" s="4" t="s">
         <v>17</v>
       </c>
@@ -3658,13 +3698,13 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="K32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L32" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="L32" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="2:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B33" s="4" t="s">
         <v>18</v>
       </c>
@@ -3681,10 +3721,10 @@
         <v>17</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B34" s="4" t="s">
         <v>42</v>
       </c>
@@ -3701,10 +3741,10 @@
         <v>18</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B35" s="4" t="s">
         <v>43</v>
       </c>
@@ -3733,12 +3773,12 @@
         <v>42</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B36" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -3751,64 +3791,64 @@
         <v>43</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B37" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C37" s="1">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="F37" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="G37" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="H37" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="I37" s="1">
         <v>7777777</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B38" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="1">
         <v>7777777</v>
       </c>
       <c r="D38" s="1">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="E38" s="1">
-        <v>4000</v>
+        <v>4</v>
       </c>
       <c r="F38" s="1">
-        <v>8000</v>
+        <v>8</v>
       </c>
       <c r="G38" s="1">
-        <v>16000</v>
+        <v>16</v>
       </c>
       <c r="H38" s="1">
-        <v>32000</v>
+        <v>32</v>
       </c>
       <c r="I38" s="1">
-        <v>64000</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B39" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39" s="1">
         <v>128</v>
@@ -3852,31 +3892,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="14.65" x14ac:dyDescent="0.5">
       <c r="B3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="2:3" ht="14.65" x14ac:dyDescent="0.5">
+      <c r="B4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>